<commit_message>
Data updates for new 3.3.1 transport files
</commit_message>
<xml_diff>
--- a/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
+++ b/InputData/trans/AVLRaPTC/Annual Vehicle Licensing Registration and Property Tax Costs.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeff Rissman\CodeRepositories\eps-us\InputData\trans\AVLRaPTC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-mexico\InputData\trans\AVLRaPTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D32A06-ED03-485E-BDB4-2BF12EEC6254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D735F44-3E35-4BD2-B1C5-CEAE4862EF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33735" yWindow="675" windowWidth="21600" windowHeight="22305" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{AF599D04-C13D-45D7-BEF0-770B4B16FC27}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="AVLRaPTC" sheetId="2" r:id="rId2"/>
+    <sheet name="Data" sheetId="3" r:id="rId2"/>
+    <sheet name="AVLRaPTC" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Sources:</t>
   </si>
@@ -43,36 +47,9 @@
     <t>Data</t>
   </si>
   <si>
-    <t>American Automobile Association</t>
-  </si>
-  <si>
-    <t>https://www.aaa.com/autorepair/articles/average-annual-cost-of-new-vehicle-ownership</t>
-  </si>
-  <si>
-    <t>Average Annual Cost of New Car Ownership Increases 5% to $9,282</t>
-  </si>
-  <si>
-    <t>Explanation and Examples of U.S. State Vehicle Property Taxes</t>
-  </si>
-  <si>
-    <t>Hendrickson, V. L.</t>
-  </si>
-  <si>
-    <t>Which U.S. States Charge Property Taxes for Cars?</t>
-  </si>
-  <si>
-    <t>https://www.mansionglobal.com/articles/which-u-s-states-charge-property-taxes-for-cars-220298</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>The AAA document cited above lists the average U.S.-wide annual cost of licensing, registration, and taxes as:</t>
-  </si>
-  <si>
-    <t>2019 USD/year</t>
-  </si>
-  <si>
     <t>This might seem high if one is familiar with annual license plate and car registration fees in some states,</t>
   </si>
   <si>
@@ -97,9 +74,6 @@
     <t>Currency Conversion</t>
   </si>
   <si>
-    <t>2019 to 2021 USD</t>
-  </si>
-  <si>
     <t>2012 USD/year</t>
   </si>
   <si>
@@ -140,6 +114,105 @@
   </si>
   <si>
     <t>AVLRaPTC Annual Vehicle Licensing Registration and Property Tax Costs</t>
+  </si>
+  <si>
+    <t>SEMOVI</t>
+  </si>
+  <si>
+    <t>Department of Mobility of Mexico City</t>
+  </si>
+  <si>
+    <t>Trámites y Servicios / Vehículos Particulares / Licencias y Permisos</t>
+  </si>
+  <si>
+    <t>https://www.semovi.cdmx.gob.mx/tramites-y-servicios/vehiculos-particulares/automovil/licencias/licencia-expedicion-nueva</t>
+  </si>
+  <si>
+    <t>2019 to 2012 USD</t>
+  </si>
+  <si>
+    <t>USD/MXN consistent with model) 2019</t>
+  </si>
+  <si>
+    <t>2022 MXN (current)</t>
+  </si>
+  <si>
+    <t>2019 USD</t>
+  </si>
+  <si>
+    <t>2012 USD</t>
+  </si>
+  <si>
+    <t>Mexico city costs</t>
+  </si>
+  <si>
+    <t>Passenger LDV</t>
+  </si>
+  <si>
+    <t>2022 MXN</t>
+  </si>
+  <si>
+    <t>Lifespan</t>
+  </si>
+  <si>
+    <t>annualized property cost</t>
+  </si>
+  <si>
+    <t>Licence</t>
+  </si>
+  <si>
+    <t>every 3 years</t>
+  </si>
+  <si>
+    <t>Plates</t>
+  </si>
+  <si>
+    <t>once</t>
+  </si>
+  <si>
+    <t>Cancel plates</t>
+  </si>
+  <si>
+    <t>Registration (t.circulación)</t>
+  </si>
+  <si>
+    <t>every 5 years</t>
+  </si>
+  <si>
+    <t>Auto tax (tenencia y refrendo)</t>
+  </si>
+  <si>
+    <t>every year</t>
+  </si>
+  <si>
+    <t>Emissions verification</t>
+  </si>
+  <si>
+    <t>twice a year</t>
+  </si>
+  <si>
+    <t>Passenger HDV</t>
+  </si>
+  <si>
+    <t>Revista</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>Motorcycles</t>
+  </si>
+  <si>
+    <t>Cargo LDV</t>
+  </si>
+  <si>
+    <t>Cargo HDV</t>
+  </si>
+  <si>
+    <t>Concession sign-in</t>
+  </si>
+  <si>
+    <t>Concession</t>
   </si>
 </sst>
 </file>
@@ -149,7 +222,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +242,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,19 +289,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="6" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -229,11 +304,22 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="3" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink 2" xfId="2" xr:uid="{37154EAF-EEE9-432C-9132-761A10D61FAB}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{C94E0D64-0F7B-422D-86FA-DE237AA379F6}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -246,6 +332,31 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="AVLRaPTC"/>
+      <sheetName val="AVPC"/>
+      <sheetName val="FpUCD"/>
+      <sheetName val="AVIC"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="66">
+          <cell r="A66">
+            <v>0.89800000000000002</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -545,194 +656,975 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC3CD7F-A224-4C3A-9A5E-D38F07B136AE}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="B11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
-        <v>2020</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B16" s="7"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="B17" s="7"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="7"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>2</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>753</v>
-      </c>
-      <c r="B17" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
+      <c r="B25" s="7"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="9">
-        <v>2</v>
-      </c>
-      <c r="B31" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="9">
-        <v>1</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="B36" t="s">
-        <v>20</v>
-      </c>
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{40391687-33E8-4157-BFF1-4B9C3152973E}"/>
-    <hyperlink ref="B13" r:id="rId2" xr:uid="{ACA01131-F87A-4018-B151-91F58C3F8660}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CE54AB-A372-4BD4-83AD-1469047EB819}">
+  <dimension ref="A1:J35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="12">
+        <v>18</v>
+      </c>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="12">
+        <v>945</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F5" s="7">
+        <v>15</v>
+      </c>
+      <c r="G5" s="7">
+        <f>SUMPRODUCT(C5:C10,E5:E10)</f>
+        <v>2356.4666666666667</v>
+      </c>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7">
+        <f>G5/$I$2</f>
+        <v>130.9148148148148</v>
+      </c>
+      <c r="J5" s="7">
+        <f>I5*[1]AVLRaPTC!$A$66</f>
+        <v>117.56150370370369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="12">
+        <v>800</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="13">
+        <f>1/F5</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="12">
+        <v>488</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="13">
+        <f>1/F5</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="12">
+        <v>358</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="13">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="12">
+        <v>628</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="12">
+        <v>628</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2553</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="13">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F12" s="7">
+        <v>20</v>
+      </c>
+      <c r="G12" s="7">
+        <f>SUMPRODUCT(C12:C14,E12:E14)</f>
+        <v>1247.4000000000001</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7">
+        <f>G12/$I$2</f>
+        <v>69.300000000000011</v>
+      </c>
+      <c r="J12" s="7">
+        <f>I12*[1]AVLRaPTC!$A$66</f>
+        <v>62.231400000000015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="12">
+        <v>822</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="13">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="12">
+        <v>232</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="12">
+        <v>473</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="13">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F16" s="7">
+        <v>15</v>
+      </c>
+      <c r="G16" s="7">
+        <f>SUMPRODUCT(C16:C19,E16:E19)</f>
+        <v>270.26666666666665</v>
+      </c>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7">
+        <f>G16/$I$2</f>
+        <v>15.014814814814814</v>
+      </c>
+      <c r="J16" s="7">
+        <f>I16*[1]AVLRaPTC!$A$66</f>
+        <v>13.483303703703703</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="12">
+        <v>586</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="13">
+        <f>1/F16</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="12">
+        <v>401</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="13">
+        <f>1/F16</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" s="12">
+        <v>234</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="13">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="12">
+        <v>945</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="13">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F22" s="7">
+        <v>10</v>
+      </c>
+      <c r="G22" s="7">
+        <f>SUMPRODUCT(C22:C27,E22:E27)</f>
+        <v>2399.4</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7">
+        <f>G22/$I$2</f>
+        <v>133.30000000000001</v>
+      </c>
+      <c r="J22" s="7">
+        <f>I22*[1]AVLRaPTC!$A$66</f>
+        <v>119.70340000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="12">
+        <v>800</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="13">
+        <f>1/F22</f>
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="12">
+        <v>488</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="13">
+        <f>1/F22</f>
+        <v>0.1</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="12">
+        <v>358</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="13">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" s="12">
+        <v>628</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="12">
+        <v>628</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="13">
+        <v>2</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="12">
+        <v>2553</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="13">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F29" s="7">
+        <v>20</v>
+      </c>
+      <c r="G29" s="7">
+        <f>SUMPRODUCT(C29:C35,E29:E35)</f>
+        <v>26393.7</v>
+      </c>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7">
+        <f>G29/$I$2</f>
+        <v>1466.3166666666666</v>
+      </c>
+      <c r="J29" s="7">
+        <f>I29*[1]AVLRaPTC!$A$66</f>
+        <v>1316.7523666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="13">
+        <f>1/F29</f>
+        <v>0.05</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="12">
+        <v>590</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="13">
+        <f>1/F29</f>
+        <v>0.05</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32" s="12">
+        <v>1246</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="13">
+        <f>1/5</f>
+        <v>0.2</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="12">
+        <v>232</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="13">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="12">
+        <v>1586</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="13">
+        <v>2</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C35" s="12">
+        <v>21860</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E35" s="7">
+        <f>1/1</f>
+        <v>1</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0F4B8D-70F0-48E9-8C0A-87C272523328}">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -741,45 +1633,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>23</v>
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="8">
-        <f>About!A17*About!$A$36</f>
-        <v>676.19399999999996</v>
-      </c>
-      <c r="C2" s="8">
-        <f>$B$2*About!$A$32</f>
-        <v>676.19399999999996</v>
+        <v>14</v>
+      </c>
+      <c r="B2" s="4">
+        <f>Data!J5</f>
+        <v>117.56150370370369</v>
+      </c>
+      <c r="C2" s="4">
+        <f>Data!J22</f>
+        <v>119.70340000000002</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="8">
-        <f>$B$2*About!$A$31</f>
-        <v>1352.3879999999999</v>
-      </c>
-      <c r="C3" s="8">
-        <f>$B$2*About!$A$31</f>
-        <v>1352.3879999999999</v>
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <f>Data!J12</f>
+        <v>62.231400000000015</v>
+      </c>
+      <c r="C3" s="4">
+        <f>Data!J29</f>
+        <v>1316.7523666666666</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -790,7 +1682,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -801,7 +1693,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -812,11 +1704,11 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="8">
-        <f>$B$2*About!$A$30</f>
-        <v>338.09699999999998</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="4">
+        <f>Data!J16</f>
+        <v>13.483303703703703</v>
       </c>
       <c r="C7">
         <v>0</v>

</xml_diff>